<commit_message>
Update README and create a vignette from it
</commit_message>
<xml_diff>
--- a/inst/extdata/examples.xlsx
+++ b/inst/extdata/examples.xlsx
@@ -150,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="123">
   <si>
     <t>normal</t>
   </si>
@@ -403,9 +403,6 @@
     <t>A cell that is not 'protected'</t>
   </si>
   <si>
-    <t>Contains a formula</t>
-  </si>
-  <si>
     <t>Text is formatted the colour 'Background1' from the theme, i.e. white.</t>
   </si>
   <si>
@@ -610,13 +607,22 @@
     <t>A cell that is 'locked'</t>
   </si>
   <si>
-    <t>String embedded in a formula</t>
-  </si>
-  <si>
     <t>Slanted text</t>
   </si>
   <si>
     <t>formula that refers to another file</t>
+  </si>
+  <si>
+    <t>formula evaluating to a number</t>
+  </si>
+  <si>
+    <t>formula evaluating to a string</t>
+  </si>
+  <si>
+    <t>formula evaluating to logical</t>
+  </si>
+  <si>
+    <t>formula evaluating to date</t>
   </si>
 </sst>
 </file>
@@ -1216,7 +1222,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1300,13 +1306,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="5" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="justify" justifyLastLine="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="justify" justifyLastLine="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -1383,11 +1390,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="273352576"/>
-        <c:axId val="273354112"/>
+        <c:axId val="273885056"/>
+        <c:axId val="273886592"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="273352576"/>
+        <c:axId val="273885056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1396,7 +1403,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="273354112"/>
+        <c:crossAx val="273886592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1404,7 +1411,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="273354112"/>
+        <c:axId val="273886592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1415,7 +1422,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="273352576"/>
+        <c:crossAx val="273885056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1779,10 +1786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B90"/>
+  <dimension ref="A1:B92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1797,7 +1804,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1805,7 +1812,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1813,7 +1820,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1858,18 +1865,18 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10" t="s">
         <v>110</v>
-      </c>
-      <c r="B10" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -1877,7 +1884,7 @@
         <v>100</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -1885,7 +1892,7 @@
         <v>0.2</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -1893,588 +1900,606 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="A14" t="b">
+        <f>1=1</f>
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15">
         <f>A4+1</f>
         <v>1338</v>
       </c>
-      <c r="B14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="str">
+      <c r="B15" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="75">
+        <f>DATE(2017,1,18)</f>
+        <v>42753</v>
+      </c>
+      <c r="B16" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="str">
         <f>"Hello, World!"</f>
         <v>Hello, World!</v>
       </c>
-      <c r="B15" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>1</v>
-      </c>
-      <c r="B16" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <f>A16+1</f>
-        <v>2</v>
-      </c>
-      <c r="B17">
-        <f>A16+2</f>
-        <v>3</v>
+      <c r="B17" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
-        <f>A17+1</f>
-        <v>3</v>
-      </c>
-      <c r="B18">
-        <f>A17+2</f>
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <f>A18+1</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B19">
         <f>A18+2</f>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="e">
-        <f t="array" ref="A20">SUM(#REF!*#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B20" t="s">
-        <v>82</v>
+      <c r="A20">
+        <f t="shared" ref="A20:A21" si="0">A19+1</f>
+        <v>3</v>
+      </c>
+      <c r="B20">
+        <f t="shared" ref="B20:B21" si="1">A19+2</f>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
-        <f t="array" ref="A21:A22">A17:A18*B17:B18</f>
-        <v>6</v>
-      </c>
-      <c r="B21" t="s">
-        <v>83</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
+        <f t="array" ref="A22">SUM(A19:A21*B19:B21)</f>
+        <v>38</v>
+      </c>
+      <c r="B22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <f t="array" ref="A23:A24">A19:A20*B19:B20</f>
+        <v>6</v>
+      </c>
+      <c r="B23" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
         <v>12</v>
       </c>
-      <c r="B22" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="str">
+      <c r="B24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="str">
         <f>[1]Sheet1!$A$1</f>
         <v>normal</v>
       </c>
-      <c r="B23" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="B25" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>0</v>
       </c>
-      <c r="B24" s="71" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="41" t="s">
+      <c r="B26" s="71" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B27" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="65" t="s">
+    <row r="28" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B28" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>0</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B29" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="64" t="s">
+    <row r="30" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B30" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+    <row r="31" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B31" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A30" s="9" t="s">
+    <row r="32" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A32" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B32" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="21" t="s">
+    <row r="33" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B31" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
+      <c r="B33" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B34" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
+    <row r="35" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B35" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="7" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B36" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="13" t="s">
+    <row r="37" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B37" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="55.5" x14ac:dyDescent="0.2">
-      <c r="A36" s="12" t="s">
+    <row r="38" spans="1:2" ht="55.5" x14ac:dyDescent="0.2">
+      <c r="A38" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B36" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="54" t="s">
+      <c r="B38" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B37" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="75.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="55" t="s">
+      <c r="B39" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="75.75" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="B38" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="72" t="s">
+      <c r="B40" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="74" t="s">
+        <v>112</v>
+      </c>
+      <c r="B41" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="74"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B43" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="72" t="s">
         <v>113</v>
       </c>
-      <c r="B39" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="72"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B41" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="73" t="s">
+      <c r="B44" t="s">
         <v>114</v>
       </c>
-      <c r="B42" t="s">
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="73" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="74" t="s">
+      <c r="B45" t="s">
         <v>116</v>
       </c>
-      <c r="B43" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="11" t="s">
+    </row>
+    <row r="46" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A46" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B46" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B45" t="s">
+    <row r="48" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B48" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B46" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="19" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B49" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B50" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="B48" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A49" s="56" t="s">
-        <v>32</v>
-      </c>
-      <c r="B49" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A50" s="56" t="s">
-        <v>32</v>
-      </c>
-      <c r="B50" s="67" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="B51" s="68" t="s">
-        <v>64</v>
+      <c r="B51" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="B52" s="69" t="s">
-        <v>65</v>
+      <c r="B52" s="67" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A53" s="57" t="s">
+      <c r="A53" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="B53" s="66" t="s">
-        <v>62</v>
+      <c r="B53" s="68" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A54" s="42" t="s">
+      <c r="A54" s="56" t="s">
+        <v>32</v>
+      </c>
+      <c r="B54" s="69" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A55" s="57" t="s">
+        <v>32</v>
+      </c>
+      <c r="B55" s="66" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A56" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="B54" s="70" t="s">
+      <c r="B56" s="70" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A57" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="B57" s="70" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A55" s="43" t="s">
-        <v>15</v>
-      </c>
-      <c r="B55" s="70" t="s">
+    <row r="58" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A58" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="B58" s="70" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A56" s="44" t="s">
-        <v>17</v>
-      </c>
-      <c r="B56" s="70" t="s">
+    <row r="59" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A59" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="B59" s="70" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A57" s="45" t="s">
-        <v>18</v>
-      </c>
-      <c r="B57" s="70" t="s">
+    <row r="60" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A60" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="B60" s="70" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A58" s="46" t="s">
-        <v>19</v>
-      </c>
-      <c r="B58" s="70" t="s">
+    <row r="61" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A61" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="B61" s="70" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A59" s="47" t="s">
-        <v>20</v>
-      </c>
-      <c r="B59" s="70" t="s">
+    <row r="62" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A62" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="B62" s="70" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A60" s="48" t="s">
-        <v>21</v>
-      </c>
-      <c r="B60" s="70" t="s">
+    <row r="63" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A63" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="B63" s="70" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A61" s="49" t="s">
-        <v>22</v>
-      </c>
-      <c r="B61" s="70" t="s">
+    <row r="64" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A64" s="50" t="s">
+        <v>23</v>
+      </c>
+      <c r="B64" s="70" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A62" s="50" t="s">
-        <v>23</v>
-      </c>
-      <c r="B62" s="70" t="s">
+    <row r="65" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A65" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="B65" s="70" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A66" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="B66" s="70" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A63" s="51" t="s">
-        <v>24</v>
-      </c>
-      <c r="B63" s="70" t="s">
+    <row r="67" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A67" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="B67" s="70" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A64" s="52" t="s">
-        <v>25</v>
-      </c>
-      <c r="B64" s="70" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A65" s="53" t="s">
-        <v>26</v>
-      </c>
-      <c r="B65" s="70" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66" s="40"/>
-      <c r="B66" t="s">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="40"/>
+      <c r="B68" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="22"/>
+      <c r="B69" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A67" s="22"/>
-      <c r="B67" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="23"/>
+      <c r="B70" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A68" s="23"/>
-      <c r="B68" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="24"/>
+      <c r="B71" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69" s="24"/>
-      <c r="B69" t="s">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="25"/>
+      <c r="B72" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A70" s="25"/>
-      <c r="B70" t="s">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="26"/>
+      <c r="B73" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A71" s="26"/>
-      <c r="B71" t="s">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" s="27"/>
+      <c r="B74" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A72" s="27"/>
-      <c r="B72" t="s">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="28"/>
+      <c r="B75" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A73" s="28"/>
-      <c r="B73" t="s">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" s="29"/>
+      <c r="B76" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A74" s="29"/>
-      <c r="B74" t="s">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" s="30"/>
+      <c r="B77" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A75" s="30"/>
-      <c r="B75" t="s">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="31"/>
+      <c r="B78" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A76" s="31"/>
-      <c r="B76" t="s">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" s="32"/>
+      <c r="B79" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A77" s="32"/>
-      <c r="B77" t="s">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="33"/>
+      <c r="B80" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A78" s="33"/>
-      <c r="B78" t="s">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="34"/>
+      <c r="B81" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A79" s="34"/>
-      <c r="B79" t="s">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="35"/>
+      <c r="B82" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A80" s="35"/>
-      <c r="B80" t="s">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="36"/>
+      <c r="B83" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" s="36"/>
-      <c r="B81" t="s">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="37"/>
+      <c r="B84" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" s="37"/>
-      <c r="B82" t="s">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="38"/>
+      <c r="B85" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="38"/>
-      <c r="B83" t="s">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="39"/>
+      <c r="B86" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="39"/>
-      <c r="B84" t="s">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="58"/>
+      <c r="B87" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" s="59"/>
+      <c r="B88" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" s="58"/>
-      <c r="B85" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" s="59"/>
-      <c r="B86" t="s">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="60"/>
+      <c r="B89" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" s="60"/>
-      <c r="B87" t="s">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" s="61"/>
+      <c r="B90" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A88" s="61"/>
-      <c r="B88" t="s">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="62"/>
+      <c r="B91" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" s="62"/>
-      <c r="B89" t="s">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" s="63"/>
+      <c r="B92" t="s">
         <v>107</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90" s="63"/>
-      <c r="B90" t="s">
-        <v>108</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A41:A42"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A63" r:id="rId1"/>
-    <hyperlink ref="A64" r:id="rId2"/>
+    <hyperlink ref="A65" r:id="rId1"/>
+    <hyperlink ref="A66" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
Improve cell description in examples.xlsx
</commit_message>
<xml_diff>
--- a/inst/extdata/examples.xlsx
+++ b/inst/extdata/examples.xlsx
@@ -589,9 +589,6 @@
     <t>comment with formatting</t>
   </si>
   <si>
-    <t>Cell A17 merged into cell 18.</t>
-  </si>
-  <si>
     <t>merged</t>
   </si>
   <si>
@@ -623,6 +620,9 @@
   </si>
   <si>
     <t>formula evaluating to date</t>
+  </si>
+  <si>
+    <t>Cell merged into cell below</t>
   </si>
 </sst>
 </file>
@@ -1310,10 +1310,10 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="justify" justifyLastLine="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -1390,11 +1390,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="273885056"/>
-        <c:axId val="273886592"/>
+        <c:axId val="129909120"/>
+        <c:axId val="129910656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="273885056"/>
+        <c:axId val="129909120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1403,7 +1403,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="273886592"/>
+        <c:crossAx val="129910656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1411,7 +1411,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="273886592"/>
+        <c:axId val="129910656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1422,7 +1422,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="273885056"/>
+        <c:crossAx val="129909120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1788,8 +1788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1909,7 +1909,7 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -1918,16 +1918,16 @@
         <v>1338</v>
       </c>
       <c r="B15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="75">
+      <c r="A16" s="74">
         <f>DATE(2017,1,18)</f>
         <v>42753</v>
       </c>
       <c r="B16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -1936,7 +1936,7 @@
         <v>Hello, World!</v>
       </c>
       <c r="B17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -2009,7 +2009,7 @@
         <v>normal</v>
       </c>
       <c r="B25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -2129,19 +2129,19 @@
         <v>7</v>
       </c>
       <c r="B40" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="74" t="s">
-        <v>112</v>
+      <c r="A41" s="75" t="s">
+        <v>111</v>
       </c>
       <c r="B41" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="74"/>
+      <c r="A42" s="75"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="10" t="s">
@@ -2153,18 +2153,18 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="72" t="s">
+        <v>112</v>
+      </c>
+      <c r="B44" t="s">
         <v>113</v>
-      </c>
-      <c r="B44" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="73" t="s">
+        <v>114</v>
+      </c>
+      <c r="B45" t="s">
         <v>115</v>
-      </c>
-      <c r="B45" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Propogate shared formulas with relative references (fixes #7)
* Introduces a dependency on
  [piton](https://cran.r-project.org/web/packages/piton/index.html), which wraps
  the [PEGTL](https://github.com/taocpp/PEGTL) parser generator.
* Parses shared formulas into tokens of types REF, TEXT, and OTHER, of which the
  only interesting type is REF, which must be offset to reconstruct related
  formulas.
* Clever enough to handle LOG10 being a valid cell reference but LOG10(1) being
  a function.
</commit_message>
<xml_diff>
--- a/inst/extdata/examples.xlsx
+++ b/inst/extdata/examples.xlsx
@@ -150,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="131">
   <si>
     <t>normal</t>
   </si>
@@ -624,15 +624,41 @@
   <si>
     <t>Cell merged into cell below</t>
   </si>
+  <si>
+    <t>custom style with custom date format</t>
+  </si>
+  <si>
+    <t>unicode shrug</t>
+  </si>
+  <si>
+    <t>¯\_(ツ)_/¯</t>
+  </si>
+  <si>
+    <t>custom number format with 'd' in [Red] to confuse date detection heuristic</t>
+  </si>
+  <si>
+    <t>ref error by deleting the reference</t>
+  </si>
+  <si>
+    <t>Test formula parser with =LOG10(1)</t>
+  </si>
+  <si>
+    <t>Test formula parser with =LOG10</t>
+  </si>
+  <si>
+    <t>Test formula parser with =C1&amp;"C1"""</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="[$-1409]d\ mmmm\ yyyy;@"/>
     <numFmt numFmtId="165" formatCode="yyyy\ mmmm\ dddd"/>
     <numFmt numFmtId="166" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="168" formatCode="\$#,##0.00;[Red]\-\$#,##0.00"/>
   </numFmts>
   <fonts count="36" x14ac:knownFonts="1">
     <font>
@@ -1214,15 +1240,15 @@
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1242,7 +1268,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2">
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="2">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
@@ -1290,8 +1316,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="5" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="5" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
@@ -1300,18 +1326,19 @@
     <xf numFmtId="0" fontId="0" fillId="29" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="5" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="5" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="5" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="justify" justifyLastLine="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -1321,7 +1348,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Normal 2" xfId="5"/>
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
-    <cellStyle name="stylealign" xfId="2"/>
+    <cellStyle name="styledate" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1390,11 +1417,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="129909120"/>
-        <c:axId val="129910656"/>
+        <c:axId val="126757888"/>
+        <c:axId val="130028288"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="129909120"/>
+        <c:axId val="126757888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1403,7 +1430,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="129910656"/>
+        <c:crossAx val="130028288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1411,7 +1438,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="129910656"/>
+        <c:axId val="130028288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1422,7 +1449,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="129909120"/>
+        <c:crossAx val="126757888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1442,7 +1469,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="126" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="129" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1453,7 +1480,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9305774" cy="6077857"/>
+    <xdr:ext cx="9310872" cy="6084186"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -1786,10 +1813,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B92"/>
+  <dimension ref="A1:B105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1949,7 +1976,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
-        <f>A18+1</f>
+        <f>$A$18+1</f>
         <v>2</v>
       </c>
       <c r="B19">
@@ -1959,8 +1986,8 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
-        <f t="shared" ref="A20:A21" si="0">A19+1</f>
-        <v>3</v>
+        <f t="shared" ref="A20:A21" si="0">$A$18+1</f>
+        <v>2</v>
       </c>
       <c r="B20">
         <f t="shared" ref="B20:B21" si="1">A19+2</f>
@@ -1970,17 +1997,17 @@
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B21">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
         <f t="array" ref="A22">SUM(A19:A21*B19:B21)</f>
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
         <v>81</v>
@@ -1997,7 +2024,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B24" t="s">
         <v>82</v>
@@ -2069,437 +2096,533 @@
       </c>
     </row>
     <row r="33" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="21" t="s">
+      <c r="A33" s="13">
+        <v>61</v>
+      </c>
+      <c r="B33" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
+    <row r="35" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
+    <row r="36" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="7" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="13" t="s">
+    <row r="38" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="55.5" x14ac:dyDescent="0.2">
-      <c r="A38" s="12" t="s">
+    <row r="39" spans="1:2" ht="55.5" x14ac:dyDescent="0.2">
+      <c r="A39" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="54" t="s">
+    <row r="40" spans="1:2" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="75.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="55" t="s">
+    <row r="41" spans="1:2" ht="75.75" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="75" t="s">
+    <row r="42" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="76" t="s">
         <v>111</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="75"/>
-    </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="10" t="s">
+      <c r="A43" s="76"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="72" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="72" t="s">
         <v>112</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="73" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="73" t="s">
         <v>114</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="11" t="s">
+    <row r="47" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47" s="15" t="s">
+    <row r="48" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" s="14" t="s">
+    <row r="49" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A49" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="19" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="20" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A51" s="56" t="s">
-        <v>32</v>
-      </c>
-      <c r="B51" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="B52" s="67" t="s">
-        <v>62</v>
+      <c r="B52" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="B53" s="68" t="s">
-        <v>63</v>
+      <c r="B53" s="67" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="B54" s="69" t="s">
+      <c r="B54" s="68" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A55" s="56" t="s">
+        <v>32</v>
+      </c>
+      <c r="B55" s="69" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A55" s="57" t="s">
+    <row r="56" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A56" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="B55" s="66" t="s">
+      <c r="B56" s="66" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A56" s="42" t="s">
+    <row r="57" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A57" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="B56" s="70" t="s">
+      <c r="B57" s="70" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A57" s="43" t="s">
+    <row r="58" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A58" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="B57" s="70" t="s">
+      <c r="B58" s="70" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A58" s="44" t="s">
+    <row r="59" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A59" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="B58" s="70" t="s">
+      <c r="B59" s="70" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A59" s="45" t="s">
+    <row r="60" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A60" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="B59" s="70" t="s">
+      <c r="B60" s="70" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A60" s="46" t="s">
+    <row r="61" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A61" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="B60" s="70" t="s">
+      <c r="B61" s="70" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A61" s="47" t="s">
+    <row r="62" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A62" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="B61" s="70" t="s">
+      <c r="B62" s="70" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A62" s="48" t="s">
+    <row r="63" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A63" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="B62" s="70" t="s">
+      <c r="B63" s="70" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A63" s="49" t="s">
+    <row r="64" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A64" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="B63" s="70" t="s">
+      <c r="B64" s="70" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A64" s="50" t="s">
+    <row r="65" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A65" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="B64" s="70" t="s">
+      <c r="B65" s="70" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A65" s="51" t="s">
+    <row r="66" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A66" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="B65" s="70" t="s">
+      <c r="B66" s="70" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A66" s="52" t="s">
+    <row r="67" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A67" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="B66" s="70" t="s">
+      <c r="B67" s="70" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A67" s="53" t="s">
+    <row r="68" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A68" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="B67" s="70" t="s">
+      <c r="B68" s="70" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A68" s="40"/>
-      <c r="B68" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="40"/>
+      <c r="B69" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69" s="22"/>
-      <c r="B69" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="22"/>
+      <c r="B70" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A70" s="23"/>
-      <c r="B70" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="23"/>
+      <c r="B71" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A71" s="24"/>
-      <c r="B71" t="s">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="24"/>
+      <c r="B72" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A72" s="25"/>
-      <c r="B72" t="s">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="25"/>
+      <c r="B73" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A73" s="26"/>
-      <c r="B73" t="s">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" s="26"/>
+      <c r="B74" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A74" s="27"/>
-      <c r="B74" t="s">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="27"/>
+      <c r="B75" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A75" s="28"/>
-      <c r="B75" t="s">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" s="28"/>
+      <c r="B76" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A76" s="29"/>
-      <c r="B76" t="s">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" s="29"/>
+      <c r="B77" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A77" s="30"/>
-      <c r="B77" t="s">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="30"/>
+      <c r="B78" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A78" s="31"/>
-      <c r="B78" t="s">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" s="31"/>
+      <c r="B79" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A79" s="32"/>
-      <c r="B79" t="s">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="32"/>
+      <c r="B80" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A80" s="33"/>
-      <c r="B80" t="s">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="33"/>
+      <c r="B81" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" s="34"/>
-      <c r="B81" t="s">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="34"/>
+      <c r="B82" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" s="35"/>
-      <c r="B82" t="s">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="35"/>
+      <c r="B83" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="36"/>
-      <c r="B83" t="s">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="36"/>
+      <c r="B84" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="37"/>
-      <c r="B84" t="s">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="37"/>
+      <c r="B85" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" s="38"/>
-      <c r="B85" t="s">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="38"/>
+      <c r="B86" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" s="39"/>
-      <c r="B86" t="s">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="39"/>
+      <c r="B87" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" s="58"/>
-      <c r="B87" t="s">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" s="58"/>
+      <c r="B88" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A88" s="59"/>
-      <c r="B88" t="s">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="59"/>
+      <c r="B89" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" s="60"/>
-      <c r="B89" t="s">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" s="60"/>
+      <c r="B90" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90" s="61"/>
-      <c r="B90" t="s">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="61"/>
+      <c r="B91" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A91" s="62"/>
-      <c r="B91" t="s">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" s="62"/>
+      <c r="B92" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A92" s="63"/>
-      <c r="B92" t="s">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="63"/>
+      <c r="B93" t="s">
         <v>107</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>125</v>
+      </c>
+      <c r="B94" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" s="75">
+        <v>-1</v>
+      </c>
+      <c r="B95" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B96" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" t="str">
+        <f>C1&amp;"C1"""</f>
+        <v>C1"</v>
+      </c>
+      <c r="B97" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" t="str">
+        <f t="shared" ref="A98:A99" si="2">C2&amp;"C1"""</f>
+        <v>C1"</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" t="str">
+        <f t="shared" si="2"/>
+        <v>C1"</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <f>LOG10</f>
+        <v>0</v>
+      </c>
+      <c r="B100" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <f t="shared" ref="A101:A102" si="3">LOG11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <f>LOG10(1)</f>
+        <v>0</v>
+      </c>
+      <c r="B103" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <f t="shared" ref="A104:A105" si="4">LOG10(1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A42:A43"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A65" r:id="rId1"/>
-    <hyperlink ref="A66" r:id="rId2"/>
+    <hyperlink ref="A66" r:id="rId1"/>
+    <hyperlink ref="A67" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
Add xlsx_validation() for data validation rules
TODO: vignette, README
</commit_message>
<xml_diff>
--- a/inst/extdata/examples.xlsx
+++ b/inst/extdata/examples.xlsx
@@ -150,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="146">
   <si>
     <t>normal</t>
   </si>
@@ -647,6 +647,51 @@
   </si>
   <si>
     <t>Test formula parser with =C1&amp;"C1"""</t>
+  </si>
+  <si>
+    <t>Data validation, custom</t>
+  </si>
+  <si>
+    <t>Data validation, not between</t>
+  </si>
+  <si>
+    <t>Data validation, not equal to</t>
+  </si>
+  <si>
+    <t>Data validation, greater than</t>
+  </si>
+  <si>
+    <t>Data validation, less than</t>
+  </si>
+  <si>
+    <t>Data validation, greater than or equal to</t>
+  </si>
+  <si>
+    <t>Data validation, less than or equal to</t>
+  </si>
+  <si>
+    <t>Data validation, decimal, not between, disallow blank, don't show message error</t>
+  </si>
+  <si>
+    <t>Data validation, list, in-cell dropdown, warning symbol</t>
+  </si>
+  <si>
+    <t>Data validation, list, no in-cell dropdown, information symbol</t>
+  </si>
+  <si>
+    <t>Data validation, time, between</t>
+  </si>
+  <si>
+    <t>Data validation, text length, between</t>
+  </si>
+  <si>
+    <t>Data validation, whole number, between, allow blank, show message title body, show error title body</t>
+  </si>
+  <si>
+    <t>Data validation, equal to, non-contiguous reference (A115,A121:A122)</t>
+  </si>
+  <si>
+    <t>Data validation, datetime, between</t>
   </si>
 </sst>
 </file>
@@ -1417,11 +1462,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="126757888"/>
-        <c:axId val="130028288"/>
+        <c:axId val="125540224"/>
+        <c:axId val="125541760"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="126757888"/>
+        <c:axId val="125540224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1430,7 +1475,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="130028288"/>
+        <c:crossAx val="125541760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1438,7 +1483,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="130028288"/>
+        <c:axId val="125541760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1449,7 +1494,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126757888"/>
+        <c:crossAx val="125540224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1813,10 +1858,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B105"/>
+  <dimension ref="A1:B122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="A102" sqref="A102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2616,10 +2661,148 @@
         <v>0</v>
       </c>
     </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B106" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B107" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B108" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B109" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B110" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B111" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B112" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B113" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="114" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B114" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="115" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B115" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="116" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B116" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="117" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B117" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="118" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B118" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="119" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B119" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="120" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B120" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="121" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B121" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="122" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B122" t="s">
+        <v>144</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A42:A43"/>
   </mergeCells>
+  <dataValidations count="15">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="error title" error="error body" promptTitle="message title" prompt="message body" sqref="A106">
+      <formula1>0</formula1>
+      <formula2>9</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A108">
+      <formula1>$B$108</formula1>
+    </dataValidation>
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A110">
+      <formula1>42736</formula1>
+      <formula2>42744.375</formula2>
+    </dataValidation>
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A111">
+      <formula1>0</formula1>
+      <formula2>0.375</formula2>
+    </dataValidation>
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A112">
+      <formula1>0</formula1>
+      <formula2>9</formula2>
+    </dataValidation>
+    <dataValidation type="whole" operator="notBetween" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A114">
+      <formula1>0</formula1>
+      <formula2>9</formula2>
+    </dataValidation>
+    <dataValidation type="whole" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A115 A121:A122">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="notEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A116">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A117">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A119">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A120">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A118">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" operator="notBetween" sqref="A107">
+      <formula1>0</formula1>
+      <formula2>9</formula2>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A113">
+      <formula1>A113&lt;=LEN(B113)</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="A109">
+      <formula1>$B$108</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
     <hyperlink ref="A66" r:id="rId1"/>
     <hyperlink ref="A67" r:id="rId2"/>

</xml_diff>

<commit_message>
Test corner cases of ref_grammar/shared_formulas
</commit_message>
<xml_diff>
--- a/inst/extdata/examples.xlsx
+++ b/inst/extdata/examples.xlsx
@@ -10,9 +10,10 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="1~`!@#$%^&amp;()_-+={}|;&quot;'&lt;,&gt;.£¹÷¦°" sheetId="2" r:id="rId2"/>
     <sheet name="chart-not-imported" sheetId="4" r:id="rId3"/>
+    <sheet name="E09904.2" sheetId="6" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <calcPr calcId="144525"/>
 </workbook>
@@ -150,7 +151,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="148">
   <si>
     <t>normal</t>
   </si>
@@ -692,6 +693,12 @@
   </si>
   <si>
     <t>Data validation, datetime, between</t>
+  </si>
+  <si>
+    <t>Test formula parser with =A1A</t>
+  </si>
+  <si>
+    <t>Test formula parser with =E09904.2!A1</t>
   </si>
 </sst>
 </file>
@@ -1462,11 +1469,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="125540224"/>
-        <c:axId val="125541760"/>
+        <c:axId val="129815296"/>
+        <c:axId val="129816832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="125540224"/>
+        <c:axId val="129815296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1475,7 +1482,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125541760"/>
+        <c:crossAx val="129816832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1483,7 +1490,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="125541760"/>
+        <c:axId val="129816832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1494,13 +1501,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125540224"/>
+        <c:crossAx val="129815296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1858,10 +1866,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B122"/>
+  <dimension ref="A1:B128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="A126" sqref="A126:A128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2696,54 +2704,96 @@
         <v>142</v>
       </c>
     </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B113" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B114" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B115" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B116" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B117" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B118" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B119" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B120" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B121" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B122" t="s">
         <v>144</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" t="e">
+        <f>A1A</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="B123" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" t="e">
+        <f t="shared" ref="A124:A125" si="5">A1A</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" t="e">
+        <f t="shared" si="5"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <f>E09904.2!A1</f>
+        <v>0</v>
+      </c>
+      <c r="B126" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <f>E09904.2!A2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <f>E09904.2!A3</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2837,4 +2887,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implement is_range() to test whether formulas are ranges
</commit_message>
<xml_diff>
--- a/inst/extdata/examples.xlsx
+++ b/inst/extdata/examples.xlsx
@@ -15,6 +15,13 @@
   <externalReferences>
     <externalReference r:id="rId5"/>
   </externalReferences>
+  <definedNames>
+    <definedName name="intersection">Sheet1!$B:$B Sheet1!$8:$8</definedName>
+    <definedName name="named_global_formula">Sheet1!$A$129-1</definedName>
+    <definedName name="named_local_formula" localSheetId="0">MAX(Sheet1!$A$129:$A$130)+1</definedName>
+    <definedName name="named_range">Sheet1!$A$129</definedName>
+    <definedName name="sheet_beyond_chart" localSheetId="3">E09904.2!$A$1,E09904.2!$C$1</definedName>
+  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
@@ -151,7 +158,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="151">
   <si>
     <t>normal</t>
   </si>
@@ -699,6 +706,15 @@
   </si>
   <si>
     <t>Test formula parser with =E09904.2!A1</t>
+  </si>
+  <si>
+    <t>Named range</t>
+  </si>
+  <si>
+    <t>Named global formula</t>
+  </si>
+  <si>
+    <t>Named local formula</t>
   </si>
 </sst>
 </file>
@@ -1469,11 +1485,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="129815296"/>
-        <c:axId val="129816832"/>
+        <c:axId val="110319104"/>
+        <c:axId val="110320640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="129815296"/>
+        <c:axId val="110319104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1482,7 +1498,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="129816832"/>
+        <c:crossAx val="110320640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1490,7 +1506,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="129816832"/>
+        <c:axId val="110320640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1501,7 +1517,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="129815296"/>
+        <c:crossAx val="110319104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1866,11 +1882,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B128"/>
+  <dimension ref="A1:B131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="A126" sqref="A126:A128"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2794,6 +2808,32 @@
       <c r="A128">
         <f>E09904.2!A3</f>
         <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>0</v>
+      </c>
+      <c r="B129" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <f>named_global_formula</f>
+        <v>-1</v>
+      </c>
+      <c r="B130" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <f>named_local_formula</f>
+        <v>1</v>
+      </c>
+      <c r="B131" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Write vignette on data validation rules
</commit_message>
<xml_diff>
--- a/inst/extdata/examples.xlsx
+++ b/inst/extdata/examples.xlsx
@@ -158,7 +158,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="152">
   <si>
     <t>normal</t>
   </si>
@@ -715,6 +715,9 @@
   </si>
   <si>
     <t>Named local formula</t>
+  </si>
+  <si>
+    <t>some text</t>
   </si>
 </sst>
 </file>
@@ -1316,7 +1319,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1409,6 +1412,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="justify" justifyLastLine="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -1485,11 +1489,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="110319104"/>
-        <c:axId val="110320640"/>
+        <c:axId val="130421504"/>
+        <c:axId val="130423040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="110319104"/>
+        <c:axId val="130421504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1498,7 +1502,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110320640"/>
+        <c:crossAx val="130423040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1506,7 +1510,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="110320640"/>
+        <c:axId val="130423040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1517,14 +1521,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110319104"/>
+        <c:crossAx val="130421504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1884,7 +1887,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B131"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="A121" sqref="A116:A121"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2684,51 +2689,81 @@
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>0</v>
+      </c>
       <c r="B106" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>0.1</v>
+      </c>
       <c r="B107" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>139</v>
+      </c>
       <c r="B108" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>139</v>
+      </c>
       <c r="B109" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" s="74">
+        <v>42736</v>
+      </c>
       <c r="B110" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" s="77">
+        <v>0.35416666666666669</v>
+      </c>
       <c r="B111" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>151</v>
+      </c>
       <c r="B112" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>10</v>
+      </c>
       <c r="B113" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>-1</v>
+      </c>
       <c r="B114" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>0</v>
+      </c>
       <c r="B115" t="s">
         <v>144</v>
       </c>
@@ -2764,6 +2799,9 @@
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>0</v>
+      </c>
       <c r="B122" t="s">
         <v>144</v>
       </c>

</xml_diff>

<commit_message>
Import in-cell formatting (fixes #5)
The new column `character_formatted` is a list-column of data frames, one per
cell.  Each row is a substring, with the applicable formatting.  Where formats
are `NA`, the overall cell format applies.
</commit_message>
<xml_diff>
--- a/inst/extdata/examples.xlsx
+++ b/inst/extdata/examples.xlsx
@@ -197,6 +197,451 @@
   </si>
   <si>
     <r>
+      <t>in-cell-bold</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>-not-bold</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>in-cell-bold</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>-not-bold</t>
+    </r>
+  </si>
+  <si>
+    <t>background2</t>
+  </si>
+  <si>
+    <t>text1</t>
+  </si>
+  <si>
+    <t>text2</t>
+  </si>
+  <si>
+    <t>accent1</t>
+  </si>
+  <si>
+    <t>accent2</t>
+  </si>
+  <si>
+    <t>accent3</t>
+  </si>
+  <si>
+    <t>accent4</t>
+  </si>
+  <si>
+    <t>accent5</t>
+  </si>
+  <si>
+    <t>accent6</t>
+  </si>
+  <si>
+    <t>hyperlink</t>
+  </si>
+  <si>
+    <t>folhyperlink</t>
+  </si>
+  <si>
+    <t>text1-lighter50</t>
+  </si>
+  <si>
+    <t>diagonal-up</t>
+  </si>
+  <si>
+    <t>diagonal-down</t>
+  </si>
+  <si>
+    <t>auto-font</t>
+  </si>
+  <si>
+    <t>empty first row and col</t>
+  </si>
+  <si>
+    <t>This worksheet has a nasty name but can be imported nevertheless</t>
+  </si>
+  <si>
+    <t>thin</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>integer with higher-precision number formatting</t>
+  </si>
+  <si>
+    <t>default date format</t>
+  </si>
+  <si>
+    <t>Different built-in date format</t>
+  </si>
+  <si>
+    <t>custom date format</t>
+  </si>
+  <si>
+    <t>'normal' style but with local italics applied to this cell.</t>
+  </si>
+  <si>
+    <t>'normal' style but with local bold applied to this cell.</t>
+  </si>
+  <si>
+    <t>'normal' style but with local underline applied to this cell.</t>
+  </si>
+  <si>
+    <t>'normal' style but with local double underline applied to this cell.</t>
+  </si>
+  <si>
+    <t>'bad' style applied to this cell</t>
+  </si>
+  <si>
+    <t>'bad' style modified with bold font, right-and-up-aligned with an indent.</t>
+  </si>
+  <si>
+    <t>'indexed' or standard red text</t>
+  </si>
+  <si>
+    <t>Blue text from the theme</t>
+  </si>
+  <si>
+    <t>Pattern but no background, blue from theme</t>
+  </si>
+  <si>
+    <t>Custom style 'stylealign' where the style is aligned to the centre.</t>
+  </si>
+  <si>
+    <t>A cell that is not 'protected'</t>
+  </si>
+  <si>
+    <t>Text is formatted the colour 'Background1' from the theme, i.e. white.</t>
+  </si>
+  <si>
+    <t>Bold applied in inline string (not at cell level)</t>
+  </si>
+  <si>
+    <t>Bold applied at cell level</t>
+  </si>
+  <si>
+    <t>Currency format</t>
+  </si>
+  <si>
+    <t>Percent format</t>
+  </si>
+  <si>
+    <t>Scientific format</t>
+  </si>
+  <si>
+    <t>Boolean (true)</t>
+  </si>
+  <si>
+    <t>Boolean (false)</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Diagonal-up border</t>
+  </si>
+  <si>
+    <t>Diagonal-down border</t>
+  </si>
+  <si>
+    <t>Automatic font colour</t>
+  </si>
+  <si>
+    <t>dashDot</t>
+  </si>
+  <si>
+    <t>no border in adjacent cell</t>
+  </si>
+  <si>
+    <t>medium border</t>
+  </si>
+  <si>
+    <t>dashed border</t>
+  </si>
+  <si>
+    <t>various combinations of borders in adacent cells</t>
+  </si>
+  <si>
+    <t>normal' style but 'normal' has been modified from Excel's default to use Arial font</t>
+  </si>
+  <si>
+    <t>text1 theme colour</t>
+  </si>
+  <si>
+    <t>background2 theme colour</t>
+  </si>
+  <si>
+    <t>text2 theme colour</t>
+  </si>
+  <si>
+    <t>accent1 theme colour</t>
+  </si>
+  <si>
+    <t>accent2 theme colour</t>
+  </si>
+  <si>
+    <t>accent3 theme colour</t>
+  </si>
+  <si>
+    <t>accent4 theme colour</t>
+  </si>
+  <si>
+    <t>accent5 theme colour</t>
+  </si>
+  <si>
+    <t>accent6 theme colour</t>
+  </si>
+  <si>
+    <t>followed hyperlink style</t>
+  </si>
+  <si>
+    <t>hyperlink style</t>
+  </si>
+  <si>
+    <t>text1-lighter50 theme colour</t>
+  </si>
+  <si>
+    <t>some formulas that are stored in groups</t>
+  </si>
+  <si>
+    <t>Custom-height row, inline string formatting of all available kinds</t>
+  </si>
+  <si>
+    <t>single-cell array formula</t>
+  </si>
+  <si>
+    <t>multi-cell array formula</t>
+  </si>
+  <si>
+    <t>More fancy inline-string formatting</t>
+  </si>
+  <si>
+    <t>Fill Highlight automatic</t>
+  </si>
+  <si>
+    <t>Fill Solid</t>
+  </si>
+  <si>
+    <t>Fill 75% Gray</t>
+  </si>
+  <si>
+    <t>Fill 50% Gray</t>
+  </si>
+  <si>
+    <t>Fill 25% Gray</t>
+  </si>
+  <si>
+    <t>Fill 12.5% Gray</t>
+  </si>
+  <si>
+    <t>Fill 6.25% Gray</t>
+  </si>
+  <si>
+    <t>Fill Horizontal Stripe</t>
+  </si>
+  <si>
+    <t>Fill Vertical Stripe</t>
+  </si>
+  <si>
+    <t>Fill Reverse Diagonal Stripe</t>
+  </si>
+  <si>
+    <t>Fill Diagonal Stripe</t>
+  </si>
+  <si>
+    <t>Fill Diagonal Crosshatch</t>
+  </si>
+  <si>
+    <t>Fill Thick Diagonal Crosshatch</t>
+  </si>
+  <si>
+    <t>Fill Thin Horizontal Stripe</t>
+  </si>
+  <si>
+    <t>Fill Thin Vertical Stripe</t>
+  </si>
+  <si>
+    <t>Fill Thin Reverse Diagonal Stripe</t>
+  </si>
+  <si>
+    <t>Fill Thin Diagonal Stripe</t>
+  </si>
+  <si>
+    <t>Fill Thin Horizontal Crosshatch</t>
+  </si>
+  <si>
+    <t>Fill Thin Diagonal Crosshatch</t>
+  </si>
+  <si>
+    <t>Fill vertical</t>
+  </si>
+  <si>
+    <t>Fill diagonal up</t>
+  </si>
+  <si>
+    <t>Fill diagonal down</t>
+  </si>
+  <si>
+    <t>Fill from corner</t>
+  </si>
+  <si>
+    <t>Fill from center</t>
+  </si>
+  <si>
+    <t>character</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>comment with formatting</t>
+  </si>
+  <si>
+    <t>merged</t>
+  </si>
+  <si>
+    <t>unhidden</t>
+  </si>
+  <si>
+    <t>A cell that is not 'hidden'</t>
+  </si>
+  <si>
+    <t>locked</t>
+  </si>
+  <si>
+    <t>A cell that is 'locked'</t>
+  </si>
+  <si>
+    <t>Slanted text</t>
+  </si>
+  <si>
+    <t>formula that refers to another file</t>
+  </si>
+  <si>
+    <t>formula evaluating to a number</t>
+  </si>
+  <si>
+    <t>formula evaluating to a string</t>
+  </si>
+  <si>
+    <t>formula evaluating to logical</t>
+  </si>
+  <si>
+    <t>formula evaluating to date</t>
+  </si>
+  <si>
+    <t>Cell merged into cell below</t>
+  </si>
+  <si>
+    <t>custom style with custom date format</t>
+  </si>
+  <si>
+    <t>unicode shrug</t>
+  </si>
+  <si>
+    <t>¯\_(ツ)_/¯</t>
+  </si>
+  <si>
+    <t>custom number format with 'd' in [Red] to confuse date detection heuristic</t>
+  </si>
+  <si>
+    <t>ref error by deleting the reference</t>
+  </si>
+  <si>
+    <t>Test formula parser with =LOG10(1)</t>
+  </si>
+  <si>
+    <t>Test formula parser with =LOG10</t>
+  </si>
+  <si>
+    <t>Test formula parser with =C1&amp;"C1"""</t>
+  </si>
+  <si>
+    <t>Data validation, custom</t>
+  </si>
+  <si>
+    <t>Data validation, not between</t>
+  </si>
+  <si>
+    <t>Data validation, not equal to</t>
+  </si>
+  <si>
+    <t>Data validation, greater than</t>
+  </si>
+  <si>
+    <t>Data validation, less than</t>
+  </si>
+  <si>
+    <t>Data validation, greater than or equal to</t>
+  </si>
+  <si>
+    <t>Data validation, less than or equal to</t>
+  </si>
+  <si>
+    <t>Data validation, decimal, not between, disallow blank, don't show message error</t>
+  </si>
+  <si>
+    <t>Data validation, list, in-cell dropdown, warning symbol</t>
+  </si>
+  <si>
+    <t>Data validation, list, no in-cell dropdown, information symbol</t>
+  </si>
+  <si>
+    <t>Data validation, time, between</t>
+  </si>
+  <si>
+    <t>Data validation, text length, between</t>
+  </si>
+  <si>
+    <t>Data validation, whole number, between, allow blank, show message title body, show error title body</t>
+  </si>
+  <si>
+    <t>Data validation, equal to, non-contiguous reference (A115,A121:A122)</t>
+  </si>
+  <si>
+    <t>Data validation, datetime, between</t>
+  </si>
+  <si>
+    <t>Test formula parser with =A1A</t>
+  </si>
+  <si>
+    <t>Test formula parser with =E09904.2!A1</t>
+  </si>
+  <si>
+    <t>Named range</t>
+  </si>
+  <si>
+    <t>Named global formula</t>
+  </si>
+  <si>
+    <t>Named local formula</t>
+  </si>
+  <si>
+    <t>some text</t>
+  </si>
+  <si>
+    <r>
       <t>in-cell</t>
     </r>
     <r>
@@ -251,7 +696,16 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>red</t>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ed</t>
     </r>
     <r>
       <rPr>
@@ -274,451 +728,6 @@
 multilinecustomheight</t>
     </r>
   </si>
-  <si>
-    <r>
-      <t>in-cell-bold</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>-not-bold</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>in-cell-bold</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>-not-bold</t>
-    </r>
-  </si>
-  <si>
-    <t>background2</t>
-  </si>
-  <si>
-    <t>text1</t>
-  </si>
-  <si>
-    <t>text2</t>
-  </si>
-  <si>
-    <t>accent1</t>
-  </si>
-  <si>
-    <t>accent2</t>
-  </si>
-  <si>
-    <t>accent3</t>
-  </si>
-  <si>
-    <t>accent4</t>
-  </si>
-  <si>
-    <t>accent5</t>
-  </si>
-  <si>
-    <t>accent6</t>
-  </si>
-  <si>
-    <t>hyperlink</t>
-  </si>
-  <si>
-    <t>folhyperlink</t>
-  </si>
-  <si>
-    <t>text1-lighter50</t>
-  </si>
-  <si>
-    <t>diagonal-up</t>
-  </si>
-  <si>
-    <t>diagonal-down</t>
-  </si>
-  <si>
-    <t>auto-font</t>
-  </si>
-  <si>
-    <t>empty first row and col</t>
-  </si>
-  <si>
-    <t>This worksheet has a nasty name but can be imported nevertheless</t>
-  </si>
-  <si>
-    <t>thin</t>
-  </si>
-  <si>
-    <t>integer</t>
-  </si>
-  <si>
-    <t>integer with higher-precision number formatting</t>
-  </si>
-  <si>
-    <t>default date format</t>
-  </si>
-  <si>
-    <t>Different built-in date format</t>
-  </si>
-  <si>
-    <t>custom date format</t>
-  </si>
-  <si>
-    <t>'normal' style but with local italics applied to this cell.</t>
-  </si>
-  <si>
-    <t>'normal' style but with local bold applied to this cell.</t>
-  </si>
-  <si>
-    <t>'normal' style but with local underline applied to this cell.</t>
-  </si>
-  <si>
-    <t>'normal' style but with local double underline applied to this cell.</t>
-  </si>
-  <si>
-    <t>'bad' style applied to this cell</t>
-  </si>
-  <si>
-    <t>'bad' style modified with bold font, right-and-up-aligned with an indent.</t>
-  </si>
-  <si>
-    <t>'indexed' or standard red text</t>
-  </si>
-  <si>
-    <t>Blue text from the theme</t>
-  </si>
-  <si>
-    <t>Pattern but no background, blue from theme</t>
-  </si>
-  <si>
-    <t>Custom style 'stylealign' where the style is aligned to the centre.</t>
-  </si>
-  <si>
-    <t>A cell that is not 'protected'</t>
-  </si>
-  <si>
-    <t>Text is formatted the colour 'Background1' from the theme, i.e. white.</t>
-  </si>
-  <si>
-    <t>Bold applied in inline string (not at cell level)</t>
-  </si>
-  <si>
-    <t>Bold applied at cell level</t>
-  </si>
-  <si>
-    <t>Currency format</t>
-  </si>
-  <si>
-    <t>Percent format</t>
-  </si>
-  <si>
-    <t>Scientific format</t>
-  </si>
-  <si>
-    <t>Boolean (true)</t>
-  </si>
-  <si>
-    <t>Boolean (false)</t>
-  </si>
-  <si>
-    <t>Error</t>
-  </si>
-  <si>
-    <t>Diagonal-up border</t>
-  </si>
-  <si>
-    <t>Diagonal-down border</t>
-  </si>
-  <si>
-    <t>Automatic font colour</t>
-  </si>
-  <si>
-    <t>dashDot</t>
-  </si>
-  <si>
-    <t>no border in adjacent cell</t>
-  </si>
-  <si>
-    <t>medium border</t>
-  </si>
-  <si>
-    <t>dashed border</t>
-  </si>
-  <si>
-    <t>various combinations of borders in adacent cells</t>
-  </si>
-  <si>
-    <t>normal' style but 'normal' has been modified from Excel's default to use Arial font</t>
-  </si>
-  <si>
-    <t>text1 theme colour</t>
-  </si>
-  <si>
-    <t>background2 theme colour</t>
-  </si>
-  <si>
-    <t>text2 theme colour</t>
-  </si>
-  <si>
-    <t>accent1 theme colour</t>
-  </si>
-  <si>
-    <t>accent2 theme colour</t>
-  </si>
-  <si>
-    <t>accent3 theme colour</t>
-  </si>
-  <si>
-    <t>accent4 theme colour</t>
-  </si>
-  <si>
-    <t>accent5 theme colour</t>
-  </si>
-  <si>
-    <t>accent6 theme colour</t>
-  </si>
-  <si>
-    <t>followed hyperlink style</t>
-  </si>
-  <si>
-    <t>hyperlink style</t>
-  </si>
-  <si>
-    <t>text1-lighter50 theme colour</t>
-  </si>
-  <si>
-    <t>some formulas that are stored in groups</t>
-  </si>
-  <si>
-    <t>Custom-height row, inline string formatting of all available kinds</t>
-  </si>
-  <si>
-    <t>single-cell array formula</t>
-  </si>
-  <si>
-    <t>multi-cell array formula</t>
-  </si>
-  <si>
-    <t>More fancy inline-string formatting</t>
-  </si>
-  <si>
-    <t>Fill Highlight automatic</t>
-  </si>
-  <si>
-    <t>Fill Solid</t>
-  </si>
-  <si>
-    <t>Fill 75% Gray</t>
-  </si>
-  <si>
-    <t>Fill 50% Gray</t>
-  </si>
-  <si>
-    <t>Fill 25% Gray</t>
-  </si>
-  <si>
-    <t>Fill 12.5% Gray</t>
-  </si>
-  <si>
-    <t>Fill 6.25% Gray</t>
-  </si>
-  <si>
-    <t>Fill Horizontal Stripe</t>
-  </si>
-  <si>
-    <t>Fill Vertical Stripe</t>
-  </si>
-  <si>
-    <t>Fill Reverse Diagonal Stripe</t>
-  </si>
-  <si>
-    <t>Fill Diagonal Stripe</t>
-  </si>
-  <si>
-    <t>Fill Diagonal Crosshatch</t>
-  </si>
-  <si>
-    <t>Fill Thick Diagonal Crosshatch</t>
-  </si>
-  <si>
-    <t>Fill Thin Horizontal Stripe</t>
-  </si>
-  <si>
-    <t>Fill Thin Vertical Stripe</t>
-  </si>
-  <si>
-    <t>Fill Thin Reverse Diagonal Stripe</t>
-  </si>
-  <si>
-    <t>Fill Thin Diagonal Stripe</t>
-  </si>
-  <si>
-    <t>Fill Thin Horizontal Crosshatch</t>
-  </si>
-  <si>
-    <t>Fill Thin Diagonal Crosshatch</t>
-  </si>
-  <si>
-    <t>Fill vertical</t>
-  </si>
-  <si>
-    <t>Fill diagonal up</t>
-  </si>
-  <si>
-    <t>Fill diagonal down</t>
-  </si>
-  <si>
-    <t>Fill from corner</t>
-  </si>
-  <si>
-    <t>Fill from center</t>
-  </si>
-  <si>
-    <t>character</t>
-  </si>
-  <si>
-    <t>comment</t>
-  </si>
-  <si>
-    <t>comment with formatting</t>
-  </si>
-  <si>
-    <t>merged</t>
-  </si>
-  <si>
-    <t>unhidden</t>
-  </si>
-  <si>
-    <t>A cell that is not 'hidden'</t>
-  </si>
-  <si>
-    <t>locked</t>
-  </si>
-  <si>
-    <t>A cell that is 'locked'</t>
-  </si>
-  <si>
-    <t>Slanted text</t>
-  </si>
-  <si>
-    <t>formula that refers to another file</t>
-  </si>
-  <si>
-    <t>formula evaluating to a number</t>
-  </si>
-  <si>
-    <t>formula evaluating to a string</t>
-  </si>
-  <si>
-    <t>formula evaluating to logical</t>
-  </si>
-  <si>
-    <t>formula evaluating to date</t>
-  </si>
-  <si>
-    <t>Cell merged into cell below</t>
-  </si>
-  <si>
-    <t>custom style with custom date format</t>
-  </si>
-  <si>
-    <t>unicode shrug</t>
-  </si>
-  <si>
-    <t>¯\_(ツ)_/¯</t>
-  </si>
-  <si>
-    <t>custom number format with 'd' in [Red] to confuse date detection heuristic</t>
-  </si>
-  <si>
-    <t>ref error by deleting the reference</t>
-  </si>
-  <si>
-    <t>Test formula parser with =LOG10(1)</t>
-  </si>
-  <si>
-    <t>Test formula parser with =LOG10</t>
-  </si>
-  <si>
-    <t>Test formula parser with =C1&amp;"C1"""</t>
-  </si>
-  <si>
-    <t>Data validation, custom</t>
-  </si>
-  <si>
-    <t>Data validation, not between</t>
-  </si>
-  <si>
-    <t>Data validation, not equal to</t>
-  </si>
-  <si>
-    <t>Data validation, greater than</t>
-  </si>
-  <si>
-    <t>Data validation, less than</t>
-  </si>
-  <si>
-    <t>Data validation, greater than or equal to</t>
-  </si>
-  <si>
-    <t>Data validation, less than or equal to</t>
-  </si>
-  <si>
-    <t>Data validation, decimal, not between, disallow blank, don't show message error</t>
-  </si>
-  <si>
-    <t>Data validation, list, in-cell dropdown, warning symbol</t>
-  </si>
-  <si>
-    <t>Data validation, list, no in-cell dropdown, information symbol</t>
-  </si>
-  <si>
-    <t>Data validation, time, between</t>
-  </si>
-  <si>
-    <t>Data validation, text length, between</t>
-  </si>
-  <si>
-    <t>Data validation, whole number, between, allow blank, show message title body, show error title body</t>
-  </si>
-  <si>
-    <t>Data validation, equal to, non-contiguous reference (A115,A121:A122)</t>
-  </si>
-  <si>
-    <t>Data validation, datetime, between</t>
-  </si>
-  <si>
-    <t>Test formula parser with =A1A</t>
-  </si>
-  <si>
-    <t>Test formula parser with =E09904.2!A1</t>
-  </si>
-  <si>
-    <t>Named range</t>
-  </si>
-  <si>
-    <t>Named global formula</t>
-  </si>
-  <si>
-    <t>Named local formula</t>
-  </si>
-  <si>
-    <t>some text</t>
-  </si>
 </sst>
 </file>
 
@@ -731,7 +740,7 @@
     <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="168" formatCode="\$#,##0.00;[Red]\-\$#,##0.00"/>
   </numFmts>
-  <fonts count="36" x14ac:knownFonts="1">
+  <fonts count="37" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Arial"/>
@@ -994,6 +1003,12 @@
       <sz val="8"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1409,10 +1424,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="justify" justifyLastLine="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -1489,11 +1504,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="130421504"/>
-        <c:axId val="130423040"/>
+        <c:axId val="127874560"/>
+        <c:axId val="127876096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="130421504"/>
+        <c:axId val="127874560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1502,7 +1517,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="130423040"/>
+        <c:crossAx val="127876096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1510,7 +1525,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="130423040"/>
+        <c:axId val="127876096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1521,7 +1536,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="130421504"/>
+        <c:crossAx val="127874560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1887,8 +1902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="A121" sqref="A116:A121"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1903,7 +1918,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="B1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1911,7 +1926,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1919,7 +1934,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1927,7 +1942,7 @@
         <v>1337</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1935,7 +1950,7 @@
         <v>1338</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1943,7 +1958,7 @@
         <v>42046</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1951,7 +1966,7 @@
         <v>42047</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -1959,23 +1974,23 @@
         <v>42048</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" t="s">
         <v>109</v>
-      </c>
-      <c r="B10" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -1983,7 +1998,7 @@
         <v>100</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -1991,7 +2006,7 @@
         <v>0.2</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -1999,7 +2014,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -2008,7 +2023,7 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -2017,7 +2032,7 @@
         <v>1338</v>
       </c>
       <c r="B15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -2026,7 +2041,7 @@
         <v>42753</v>
       </c>
       <c r="B16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -2035,7 +2050,7 @@
         <v>Hello, World!</v>
       </c>
       <c r="B17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -2043,7 +2058,7 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -2082,7 +2097,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -2091,7 +2106,7 @@
         <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -2099,7 +2114,7 @@
         <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -2108,7 +2123,7 @@
         <v>normal</v>
       </c>
       <c r="B25" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -2116,7 +2131,7 @@
         <v>0</v>
       </c>
       <c r="B26" s="71" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -2124,7 +2139,7 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -2132,7 +2147,7 @@
         <v>0</v>
       </c>
       <c r="B28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -2140,7 +2155,7 @@
         <v>0</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -2148,7 +2163,7 @@
         <v>0</v>
       </c>
       <c r="B30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -2156,7 +2171,7 @@
         <v>2</v>
       </c>
       <c r="B31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15" x14ac:dyDescent="0.2">
@@ -2164,7 +2179,7 @@
         <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -2172,15 +2187,15 @@
         <v>61</v>
       </c>
       <c r="B33" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -2188,7 +2203,7 @@
         <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -2196,7 +2211,7 @@
         <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -2204,7 +2219,7 @@
         <v>3</v>
       </c>
       <c r="B37" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2212,15 +2227,15 @@
         <v>8</v>
       </c>
       <c r="B38" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="55.5" x14ac:dyDescent="0.2">
       <c r="A39" s="12" t="s">
-        <v>12</v>
+        <v>151</v>
       </c>
       <c r="B39" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -2228,7 +2243,7 @@
         <v>11</v>
       </c>
       <c r="B40" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="75.75" thickTop="1" x14ac:dyDescent="0.2">
@@ -2236,42 +2251,42 @@
         <v>7</v>
       </c>
       <c r="B41" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="76" t="s">
-        <v>111</v>
+      <c r="A42" s="77" t="s">
+        <v>110</v>
       </c>
       <c r="B42" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="76"/>
+      <c r="A43" s="77"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
         <v>9</v>
       </c>
       <c r="B44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="72" t="s">
+        <v>111</v>
+      </c>
+      <c r="B45" t="s">
         <v>112</v>
-      </c>
-      <c r="B45" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="73" t="s">
+        <v>113</v>
+      </c>
+      <c r="B46" t="s">
         <v>114</v>
-      </c>
-      <c r="B46" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -2279,333 +2294,333 @@
         <v>10</v>
       </c>
       <c r="B47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B48" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B49" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B50" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B51" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="56" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B52" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="56" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B53" s="67" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="56" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B54" s="68" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="56" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B55" s="69" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="57" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B56" s="66" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="42" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B57" s="70" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="43" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B58" s="70" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="44" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B59" s="70" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="45" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B60" s="70" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="46" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B61" s="70" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="47" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B62" s="70" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="48" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B63" s="70" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="49" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B64" s="70" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="50" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B65" s="70" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="51" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B66" s="70" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="52" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B67" s="70" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="53" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B68" s="70" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="40"/>
       <c r="B69" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="22"/>
       <c r="B70" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="23"/>
       <c r="B71" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="24"/>
       <c r="B72" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="25"/>
       <c r="B73" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="26"/>
       <c r="B74" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="27"/>
       <c r="B75" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="28"/>
       <c r="B76" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="29"/>
       <c r="B77" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="30"/>
       <c r="B78" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="31"/>
       <c r="B79" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="32"/>
       <c r="B80" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="33"/>
       <c r="B81" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="34"/>
       <c r="B82" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="35"/>
       <c r="B83" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="36"/>
       <c r="B84" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="37"/>
       <c r="B85" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="38"/>
       <c r="B86" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="39"/>
       <c r="B87" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="58"/>
       <c r="B88" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="59"/>
       <c r="B89" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="60"/>
       <c r="B90" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="61"/>
       <c r="B91" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="62"/>
       <c r="B92" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="63"/>
       <c r="B93" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B94" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
@@ -2613,7 +2628,7 @@
         <v>-1</v>
       </c>
       <c r="B95" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
@@ -2622,7 +2637,7 @@
         <v>#REF!</v>
       </c>
       <c r="B96" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
@@ -2631,7 +2646,7 @@
         <v>C1"</v>
       </c>
       <c r="B97" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
@@ -2652,7 +2667,7 @@
         <v>0</v>
       </c>
       <c r="B100" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
@@ -2673,7 +2688,7 @@
         <v>0</v>
       </c>
       <c r="B103" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
@@ -2693,7 +2708,7 @@
         <v>0</v>
       </c>
       <c r="B106" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
@@ -2701,23 +2716,23 @@
         <v>0.1</v>
       </c>
       <c r="B107" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B108" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
+        <v>138</v>
+      </c>
+      <c r="B109" t="s">
         <v>139</v>
-      </c>
-      <c r="B109" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
@@ -2725,23 +2740,23 @@
         <v>42736</v>
       </c>
       <c r="B110" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A111" s="77">
+      <c r="A111" s="76">
         <v>0.35416666666666669</v>
       </c>
       <c r="B111" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B112" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
@@ -2749,7 +2764,7 @@
         <v>10</v>
       </c>
       <c r="B113" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
@@ -2757,7 +2772,7 @@
         <v>-1</v>
       </c>
       <c r="B114" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
@@ -2765,37 +2780,37 @@
         <v>0</v>
       </c>
       <c r="B115" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B116" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B117" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B118" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B119" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B120" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B121" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
@@ -2803,7 +2818,7 @@
         <v>0</v>
       </c>
       <c r="B122" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
@@ -2812,7 +2827,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B123" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
@@ -2833,7 +2848,7 @@
         <v>0</v>
       </c>
       <c r="B126" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
@@ -2853,7 +2868,7 @@
         <v>0</v>
       </c>
       <c r="B129" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
@@ -2862,7 +2877,7 @@
         <v>-1</v>
       </c>
       <c r="B130" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
@@ -2871,7 +2886,7 @@
         <v>1</v>
       </c>
       <c r="B131" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -2953,12 +2968,12 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Support all in-cell formats (#5)
</commit_message>
<xml_diff>
--- a/inst/extdata/examples.xlsx
+++ b/inst/extdata/examples.xlsx
@@ -425,9 +425,6 @@
     <t>some formulas that are stored in groups</t>
   </si>
   <si>
-    <t>Custom-height row, inline string formatting of all available kinds</t>
-  </si>
-  <si>
     <t>single-cell array formula</t>
   </si>
   <si>
@@ -641,7 +638,17 @@
     <t>some text</t>
   </si>
   <si>
+    <t>in-cellbolditalicunderlineunderlinedoublesingleaccountingdoubleaccountingstrikethroughsuperscriptsubscriptredthemeaccentsizearial
+multilinecustomheight</t>
+  </si>
+  <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>in-cell</t>
     </r>
     <r>
@@ -679,33 +686,99 @@
     </r>
     <r>
       <rPr>
-        <b/>
-        <i/>
-        <u/>
+        <u val="double"/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>all-three</t>
+      <t>underlinedouble</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="singleAccounting"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>singleaccounting</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="doubleAccounting"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>doubleaccounting</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>strikethrough</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>subscript</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>superscript</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Arial"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
+        <scheme val="minor"/>
       </rPr>
-      <t>r</t>
+      <t>red</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color theme="5"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
+        <scheme val="minor"/>
       </rPr>
-      <t>ed</t>
+      <t>theme</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="0.79998168889431442"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tint</t>
     </r>
     <r>
       <rPr>
@@ -724,7 +797,17 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>arial
+      <t>arial</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>UTF8Stéphane
 multilinecustomheight</t>
     </r>
   </si>
@@ -740,7 +823,7 @@
     <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="168" formatCode="\$#,##0.00;[Red]\-\$#,##0.00"/>
   </numFmts>
-  <fonts count="37" x14ac:knownFonts="1">
+  <fonts count="42" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Arial"/>
@@ -844,16 +927,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <i/>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="8"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -1006,10 +1079,59 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="5"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u val="double"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u val="singleAccounting"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u val="doubleAccounting"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="0.79998168889431442"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="30">
@@ -1331,7 +1453,7 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="78">
@@ -1365,7 +1487,7 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
@@ -1385,19 +1507,19 @@
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
@@ -1410,8 +1532,8 @@
     <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="29" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="5" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="5" applyFont="1" applyBorder="1"/>
@@ -1504,11 +1626,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="127874560"/>
-        <c:axId val="127876096"/>
+        <c:axId val="129119360"/>
+        <c:axId val="129121280"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="127874560"/>
+        <c:axId val="129119360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1517,7 +1639,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127876096"/>
+        <c:crossAx val="129121280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1525,7 +1647,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="127876096"/>
+        <c:axId val="129121280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1536,13 +1658,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127874560"/>
+        <c:crossAx val="129119360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1556,7 +1679,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="129" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="123" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1567,7 +1690,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9310872" cy="6084186"/>
+    <xdr:ext cx="9308171" cy="6078963"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -1902,8 +2025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1979,18 +2102,18 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" t="s">
         <v>108</v>
-      </c>
-      <c r="B10" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -2023,7 +2146,7 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -2032,7 +2155,7 @@
         <v>1338</v>
       </c>
       <c r="B15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -2041,7 +2164,7 @@
         <v>42753</v>
       </c>
       <c r="B16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -2050,7 +2173,7 @@
         <v>Hello, World!</v>
       </c>
       <c r="B17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -2097,7 +2220,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -2106,7 +2229,7 @@
         <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -2114,7 +2237,7 @@
         <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -2123,7 +2246,7 @@
         <v>normal</v>
       </c>
       <c r="B25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -2187,7 +2310,7 @@
         <v>61</v>
       </c>
       <c r="B33" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -2230,12 +2353,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="55.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" ht="123.75" x14ac:dyDescent="0.2">
       <c r="A39" s="12" t="s">
         <v>151</v>
       </c>
       <c r="B39" t="s">
-        <v>79</v>
+        <v>150</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -2243,7 +2366,7 @@
         <v>11</v>
       </c>
       <c r="B40" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="75.75" thickTop="1" x14ac:dyDescent="0.2">
@@ -2251,15 +2374,15 @@
         <v>7</v>
       </c>
       <c r="B41" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="77" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B42" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -2275,18 +2398,18 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="72" t="s">
+        <v>110</v>
+      </c>
+      <c r="B45" t="s">
         <v>111</v>
-      </c>
-      <c r="B45" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="73" t="s">
+        <v>112</v>
+      </c>
+      <c r="B46" t="s">
         <v>113</v>
-      </c>
-      <c r="B46" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -2468,159 +2591,159 @@
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="40"/>
       <c r="B69" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="22"/>
       <c r="B70" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="23"/>
       <c r="B71" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="24"/>
       <c r="B72" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="25"/>
       <c r="B73" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="26"/>
       <c r="B74" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="27"/>
       <c r="B75" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="28"/>
       <c r="B76" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="29"/>
       <c r="B77" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="30"/>
       <c r="B78" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="31"/>
       <c r="B79" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="32"/>
       <c r="B80" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="33"/>
       <c r="B81" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="34"/>
       <c r="B82" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="35"/>
       <c r="B83" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="36"/>
       <c r="B84" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="37"/>
       <c r="B85" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="38"/>
       <c r="B86" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="39"/>
       <c r="B87" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="58"/>
       <c r="B88" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="59"/>
       <c r="B89" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="60"/>
       <c r="B90" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="61"/>
       <c r="B91" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="62"/>
       <c r="B92" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="63"/>
       <c r="B93" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B94" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
@@ -2628,7 +2751,7 @@
         <v>-1</v>
       </c>
       <c r="B95" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
@@ -2637,7 +2760,7 @@
         <v>#REF!</v>
       </c>
       <c r="B96" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
@@ -2646,7 +2769,7 @@
         <v>C1"</v>
       </c>
       <c r="B97" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
@@ -2667,7 +2790,7 @@
         <v>0</v>
       </c>
       <c r="B100" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
@@ -2688,7 +2811,7 @@
         <v>0</v>
       </c>
       <c r="B103" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
@@ -2708,7 +2831,7 @@
         <v>0</v>
       </c>
       <c r="B106" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
@@ -2716,23 +2839,23 @@
         <v>0.1</v>
       </c>
       <c r="B107" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B108" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
+        <v>137</v>
+      </c>
+      <c r="B109" t="s">
         <v>138</v>
-      </c>
-      <c r="B109" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
@@ -2740,7 +2863,7 @@
         <v>42736</v>
       </c>
       <c r="B110" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
@@ -2748,15 +2871,15 @@
         <v>0.35416666666666669</v>
       </c>
       <c r="B111" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B112" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
@@ -2764,7 +2887,7 @@
         <v>10</v>
       </c>
       <c r="B113" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
@@ -2772,7 +2895,7 @@
         <v>-1</v>
       </c>
       <c r="B114" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
@@ -2780,37 +2903,37 @@
         <v>0</v>
       </c>
       <c r="B115" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B116" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B117" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B118" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B119" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B120" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B121" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
@@ -2818,7 +2941,7 @@
         <v>0</v>
       </c>
       <c r="B122" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
@@ -2827,7 +2950,7 @@
         <v>#NAME?</v>
       </c>
       <c r="B123" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
@@ -2848,7 +2971,7 @@
         <v>0</v>
       </c>
       <c r="B126" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
@@ -2868,7 +2991,7 @@
         <v>0</v>
       </c>
       <c r="B129" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
@@ -2877,7 +3000,7 @@
         <v>-1</v>
       </c>
       <c r="B130" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
@@ -2886,7 +3009,7 @@
         <v>1</v>
       </c>
       <c r="B131" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add comments and hidden to xlsx_names (closes #17)
</commit_message>
<xml_diff>
--- a/inst/extdata/examples.xlsx
+++ b/inst/extdata/examples.xlsx
@@ -19,7 +19,7 @@
     <definedName name="intersection">Sheet1!$B:$B Sheet1!$8:$8</definedName>
     <definedName name="named_global_formula">Sheet1!$A$129-1</definedName>
     <definedName name="named_local_formula" localSheetId="0">MAX(Sheet1!$A$129:$A$130)+1</definedName>
-    <definedName name="named_range">Sheet1!$A$129</definedName>
+    <definedName name="named_range" comment="My comment">Sheet1!$A$129</definedName>
     <definedName name="sheet_beyond_chart" localSheetId="3">E09904.2!$A$1,E09904.2!$C$1</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
@@ -1603,10 +1603,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="justify" justifyLastLine="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -1683,11 +1683,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="127284736"/>
-        <c:axId val="127286272"/>
+        <c:axId val="128595840"/>
+        <c:axId val="128597376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="127284736"/>
+        <c:axId val="128595840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1696,7 +1696,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127286272"/>
+        <c:crossAx val="128597376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1704,7 +1704,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="127286272"/>
+        <c:axId val="128597376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1715,7 +1715,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127284736"/>
+        <c:crossAx val="128595840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2434,7 +2434,7 @@
       </c>
     </row>
     <row r="42" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="77" t="s">
+      <c r="A42" s="78" t="s">
         <v>109</v>
       </c>
       <c r="B42" t="s">
@@ -2442,7 +2442,7 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="77"/>
+      <c r="A43" s="78"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
@@ -3069,7 +3069,7 @@
       </c>
     </row>
     <row r="132" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A132" s="78" t="s">
+      <c r="A132" s="77" t="s">
         <v>153</v>
       </c>
       <c r="B132" t="s">

</xml_diff>

<commit_message>
Update examples for the recent new tests
</commit_message>
<xml_diff>
--- a/inst/extdata/examples.xlsx
+++ b/inst/extdata/examples.xlsx
@@ -11,9 +11,10 @@
     <sheet name="1~`!@#$%^&amp;()_-+={}|;&quot;'&lt;,&gt;.£¹÷¦°" sheetId="2" r:id="rId2"/>
     <sheet name="chart-not-imported" sheetId="4" r:id="rId3"/>
     <sheet name="E09904.2" sheetId="6" r:id="rId4"/>
+    <sheet name="gradientFill" sheetId="7" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <definedNames>
     <definedName name="intersection">Sheet1!$B:$B Sheet1!$8:$8</definedName>
@@ -158,7 +159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="219">
   <si>
     <t>normal</t>
   </si>
@@ -846,6 +847,201 @@
       <t xml:space="preserve"> with cell-level defaults</t>
     </r>
   </si>
+  <si>
+    <t>underline single accounting</t>
+  </si>
+  <si>
+    <t>underline double accounting</t>
+  </si>
+  <si>
+    <t>strikethrough</t>
+  </si>
+  <si>
+    <t>superscript</t>
+  </si>
+  <si>
+    <t>subscript</t>
+  </si>
+  <si>
+    <t>tint</t>
+  </si>
+  <si>
+    <t>Two-colour fill</t>
+  </si>
+  <si>
+    <t>Fill Horizontal Variant 2</t>
+  </si>
+  <si>
+    <t>Fill Horizontal Variant 3</t>
+  </si>
+  <si>
+    <t>Fill vertical variant 2</t>
+  </si>
+  <si>
+    <t>Fill vertical variant 3</t>
+  </si>
+  <si>
+    <t>Fill diagonal up variant 2</t>
+  </si>
+  <si>
+    <t>Fill diagonal up variant 3</t>
+  </si>
+  <si>
+    <t>Fill diagonal down variant 2</t>
+  </si>
+  <si>
+    <t>Fill diagonal down variant 3</t>
+  </si>
+  <si>
+    <t>Fill from corner variant 2</t>
+  </si>
+  <si>
+    <t>Fill from corner variant 3</t>
+  </si>
+  <si>
+    <t>Fill from corner variant 4</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>degree</t>
+  </si>
+  <si>
+    <t>left</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>right</t>
+  </si>
+  <si>
+    <t>top</t>
+  </si>
+  <si>
+    <t>bottom</t>
+  </si>
+  <si>
+    <t>stop1 positon</t>
+  </si>
+  <si>
+    <t>stop2 position</t>
+  </si>
+  <si>
+    <t>Fill Horizontal</t>
+  </si>
+  <si>
+    <t>hair</t>
+  </si>
+  <si>
+    <t>dotted</t>
+  </si>
+  <si>
+    <t>dashDotDot</t>
+  </si>
+  <si>
+    <t>dashed</t>
+  </si>
+  <si>
+    <t>mediumDashDotDot</t>
+  </si>
+  <si>
+    <t>slantDashDot</t>
+  </si>
+  <si>
+    <t>mediumDashDot</t>
+  </si>
+  <si>
+    <t>mediumDashed</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>thick</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>diagonalUp</t>
+  </si>
+  <si>
+    <t>diagonalDown</t>
+  </si>
+  <si>
+    <t>both diagonals (will always be the same style)</t>
+  </si>
+  <si>
+    <t>vertical align top</t>
+  </si>
+  <si>
+    <t>vertical align bottom</t>
+  </si>
+  <si>
+    <t>horizontal align left</t>
+  </si>
+  <si>
+    <t>horizontal align right</t>
+  </si>
+  <si>
+    <t>horizontal align center</t>
+  </si>
+  <si>
+    <t>indent</t>
+  </si>
+  <si>
+    <t>vertical align center</t>
+  </si>
+  <si>
+    <t>vertical align justify</t>
+  </si>
+  <si>
+    <t>vertical align distributed</t>
+  </si>
+  <si>
+    <t>horizontal align general</t>
+  </si>
+  <si>
+    <t>horizontal align fill</t>
+  </si>
+  <si>
+    <t>horizontal align justify</t>
+  </si>
+  <si>
+    <t>horizontal align center across selection</t>
+  </si>
+  <si>
+    <t>horizontal align distributed</t>
+  </si>
+  <si>
+    <t>wrap text</t>
+  </si>
+  <si>
+    <t>shrink to fit</t>
+  </si>
+  <si>
+    <t>merge cells</t>
+  </si>
+  <si>
+    <t>reading order context</t>
+  </si>
+  <si>
+    <t>reading order left to right</t>
+  </si>
+  <si>
+    <t>reading order right to left</t>
+  </si>
+  <si>
+    <t>text rotation</t>
+  </si>
+  <si>
+    <t>hidden</t>
+  </si>
+  <si>
+    <t>a cell that is 'hidden'</t>
+  </si>
 </sst>
 </file>
 
@@ -858,7 +1054,7 @@
     <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="168" formatCode="\$#,##0.00;[Red]\-\$#,##0.00"/>
   </numFmts>
-  <fonts count="45" x14ac:knownFonts="1">
+  <fonts count="52" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Arial"/>
@@ -1189,8 +1385,50 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u val="singleAccounting"/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u val="doubleAccounting"/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="30">
+  <fills count="42">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1384,8 +1622,140 @@
         </stop>
       </gradientFill>
     </fill>
+    <fill>
+      <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
+        <stop position="0">
+          <color theme="9"/>
+        </stop>
+        <stop position="1">
+          <color theme="4"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill degree="270">
+        <stop position="0">
+          <color theme="0"/>
+        </stop>
+        <stop position="1">
+          <color theme="4"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill degree="90">
+        <stop position="0">
+          <color theme="0"/>
+        </stop>
+        <stop position="0.5">
+          <color theme="4"/>
+        </stop>
+        <stop position="1">
+          <color theme="0"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill degree="180">
+        <stop position="0">
+          <color theme="0"/>
+        </stop>
+        <stop position="1">
+          <color theme="4"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill>
+        <stop position="0">
+          <color theme="0"/>
+        </stop>
+        <stop position="0.5">
+          <color theme="4"/>
+        </stop>
+        <stop position="1">
+          <color theme="0"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill degree="225">
+        <stop position="0">
+          <color theme="0"/>
+        </stop>
+        <stop position="1">
+          <color theme="4"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill degree="45">
+        <stop position="0">
+          <color theme="0"/>
+        </stop>
+        <stop position="0.5">
+          <color theme="4"/>
+        </stop>
+        <stop position="1">
+          <color theme="0"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill degree="315">
+        <stop position="0">
+          <color theme="0"/>
+        </stop>
+        <stop position="1">
+          <color theme="4"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill degree="135">
+        <stop position="0">
+          <color theme="0"/>
+        </stop>
+        <stop position="0.5">
+          <color theme="4"/>
+        </stop>
+        <stop position="1">
+          <color theme="0"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill type="path" left="1" right="1">
+        <stop position="0">
+          <color theme="0"/>
+        </stop>
+        <stop position="1">
+          <color theme="4"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill type="path" top="1" bottom="1">
+        <stop position="0">
+          <color theme="0"/>
+        </stop>
+        <stop position="1">
+          <color theme="4"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill type="path" left="1" right="1" top="1" bottom="1">
+        <stop position="0">
+          <color theme="0"/>
+        </stop>
+        <stop position="1">
+          <color theme="4"/>
+        </stop>
+      </gradientFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -1500,6 +1870,170 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dotted">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dashDotDot">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dashDot">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="mediumDashDotDot">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="slantDashDot">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="mediumDashDot">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="mediumDashed">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="1">
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal style="hair">
+        <color auto="1"/>
+      </diagonal>
+    </border>
+    <border diagonalDown="1">
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal style="hair">
+        <color auto="1"/>
+      </diagonal>
+    </border>
+    <border diagonalUp="1" diagonalDown="1">
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal style="hair">
+        <color auto="1"/>
+      </diagonal>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1512,7 +2046,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="156">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1604,9 +2138,121 @@
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="distributed"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="distributed"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment textRotation="105"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment readingOrder="2"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="justify" justifyLastLine="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -1683,11 +2329,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="128595840"/>
-        <c:axId val="128597376"/>
+        <c:axId val="128652032"/>
+        <c:axId val="128653568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="128595840"/>
+        <c:axId val="128652032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1696,7 +2342,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128597376"/>
+        <c:crossAx val="128653568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1704,7 +2350,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="128597376"/>
+        <c:axId val="128653568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1715,7 +2361,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128595840"/>
+        <c:crossAx val="128652032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1735,7 +2381,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="123" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="96" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1746,7 +2392,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9308171" cy="6078963"/>
+    <xdr:ext cx="9227344" cy="6022578"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -2079,10 +2725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B132"/>
+  <dimension ref="A1:G188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="A132" sqref="A132"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="A121" activeCellId="1" sqref="A115 A121:A122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2330,7 +2976,7 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="A29" s="78" t="s">
         <v>0</v>
       </c>
       <c r="B29" t="s">
@@ -2434,7 +3080,7 @@
       </c>
     </row>
     <row r="42" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="78" t="s">
+      <c r="A42" s="154" t="s">
         <v>109</v>
       </c>
       <c r="B42" t="s">
@@ -2442,7 +3088,7 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="78"/>
+      <c r="A43" s="154"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
@@ -3076,9 +3722,436 @@
         <v>152</v>
       </c>
     </row>
+    <row r="133" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A133" s="79" t="s">
+        <v>154</v>
+      </c>
+      <c r="B133" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A134" s="80" t="s">
+        <v>155</v>
+      </c>
+      <c r="B134" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" s="81" t="s">
+        <v>156</v>
+      </c>
+      <c r="B135" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A136" s="82" t="s">
+        <v>157</v>
+      </c>
+      <c r="B136" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="A137" s="83" t="s">
+        <v>158</v>
+      </c>
+      <c r="B137" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" s="84" t="s">
+        <v>159</v>
+      </c>
+      <c r="B138" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139" s="85"/>
+      <c r="B139" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140" s="86"/>
+      <c r="B140" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" s="87"/>
+      <c r="B141" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142" s="88"/>
+      <c r="B142" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143" s="89"/>
+      <c r="B143" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144" s="90"/>
+      <c r="B144" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145" s="91"/>
+      <c r="B145" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146" s="92"/>
+      <c r="B146" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147" s="93"/>
+      <c r="B147" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148" s="94"/>
+      <c r="B148" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149" s="95"/>
+      <c r="B149" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150" s="96"/>
+      <c r="B150" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151" s="122" t="s">
+        <v>182</v>
+      </c>
+      <c r="B151" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152" s="123" t="s">
+        <v>183</v>
+      </c>
+      <c r="B152" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153" s="124" t="s">
+        <v>184</v>
+      </c>
+      <c r="B153" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A154" s="125" t="s">
+        <v>60</v>
+      </c>
+      <c r="B154" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A155" s="126" t="s">
+        <v>185</v>
+      </c>
+      <c r="B155" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A156" s="102" t="s">
+        <v>31</v>
+      </c>
+      <c r="B156" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A157" s="127" t="s">
+        <v>186</v>
+      </c>
+      <c r="B157" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A158" s="128" t="s">
+        <v>187</v>
+      </c>
+      <c r="B158" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A159" s="129" t="s">
+        <v>188</v>
+      </c>
+      <c r="B159" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A160" s="130" t="s">
+        <v>189</v>
+      </c>
+      <c r="B160" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A161" s="131" t="s">
+        <v>190</v>
+      </c>
+      <c r="B161" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A162" s="132" t="s">
+        <v>191</v>
+      </c>
+      <c r="B162" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A163" s="133" t="s">
+        <v>192</v>
+      </c>
+      <c r="B163" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A164" s="134" t="s">
+        <v>193</v>
+      </c>
+      <c r="B164" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A165" s="135" t="s">
+        <v>194</v>
+      </c>
+      <c r="B165" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A166" s="136" t="s">
+        <v>195</v>
+      </c>
+      <c r="B166" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>205</v>
+      </c>
+      <c r="B167" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A168" s="141" t="s">
+        <v>198</v>
+      </c>
+      <c r="B168" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A169" s="140" t="s">
+        <v>200</v>
+      </c>
+      <c r="B169" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A170" s="139" t="s">
+        <v>199</v>
+      </c>
+      <c r="B170" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A171" s="145" t="s">
+        <v>206</v>
+      </c>
+      <c r="B171" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A172" s="146" t="s">
+        <v>207</v>
+      </c>
+      <c r="B172" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A173" s="147" t="s">
+        <v>208</v>
+      </c>
+      <c r="B173" s="147"/>
+      <c r="D173" s="147" t="s">
+        <v>208</v>
+      </c>
+      <c r="E173" s="147"/>
+      <c r="F173" s="147"/>
+      <c r="G173" s="147"/>
+    </row>
+    <row r="174" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A174" s="148" t="s">
+        <v>209</v>
+      </c>
+      <c r="B174" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A175" s="137" t="s">
+        <v>196</v>
+      </c>
+      <c r="B175" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A176" s="138" t="s">
+        <v>202</v>
+      </c>
+      <c r="B176" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>197</v>
+      </c>
+      <c r="B177" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A178" s="143" t="s">
+        <v>203</v>
+      </c>
+      <c r="B178" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A179" s="144" t="s">
+        <v>204</v>
+      </c>
+      <c r="B179" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A180" s="142" t="s">
+        <v>201</v>
+      </c>
+      <c r="B180" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A181" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="B181" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A182" s="149" t="s">
+        <v>211</v>
+      </c>
+      <c r="B182" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A183" s="155" t="s">
+        <v>212</v>
+      </c>
+      <c r="B183" s="155"/>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>213</v>
+      </c>
+      <c r="B184" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A185" s="150" t="s">
+        <v>214</v>
+      </c>
+      <c r="B185" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A186" s="151" t="s">
+        <v>215</v>
+      </c>
+      <c r="B186" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" ht="30.75" x14ac:dyDescent="0.2">
+      <c r="A187" s="152" t="s">
+        <v>216</v>
+      </c>
+      <c r="B187" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A188" s="153" t="s">
+        <v>217</v>
+      </c>
+      <c r="B188" t="s">
+        <v>218</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A183:B183"/>
   </mergeCells>
   <dataValidations count="15">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="error title" error="error body" promptTitle="message title" prompt="message body" sqref="A106">
@@ -3179,4 +4252,453 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.25" customWidth="1"/>
+    <col min="2" max="2" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F1" t="s">
+        <v>173</v>
+      </c>
+      <c r="G1" t="s">
+        <v>174</v>
+      </c>
+      <c r="H1" t="s">
+        <v>176</v>
+      </c>
+      <c r="I1" t="s">
+        <v>177</v>
+      </c>
+      <c r="J1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="109"/>
+      <c r="B3" s="98" t="s">
+        <v>181</v>
+      </c>
+      <c r="C3" s="98">
+        <v>0</v>
+      </c>
+      <c r="D3" s="98">
+        <v>1</v>
+      </c>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98">
+        <v>90</v>
+      </c>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="99"/>
+    </row>
+    <row r="4" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="110"/>
+      <c r="B4" s="101" t="s">
+        <v>161</v>
+      </c>
+      <c r="C4" s="101">
+        <v>0</v>
+      </c>
+      <c r="D4" s="101">
+        <v>1</v>
+      </c>
+      <c r="E4" s="101"/>
+      <c r="F4" s="101">
+        <v>270</v>
+      </c>
+      <c r="G4" s="101"/>
+      <c r="H4" s="101"/>
+      <c r="I4" s="101"/>
+      <c r="J4" s="102"/>
+    </row>
+    <row r="5" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="111"/>
+      <c r="B5" s="104" t="s">
+        <v>162</v>
+      </c>
+      <c r="C5" s="104">
+        <v>0</v>
+      </c>
+      <c r="D5" s="104">
+        <v>0.5</v>
+      </c>
+      <c r="E5" s="104"/>
+      <c r="F5" s="104">
+        <v>90</v>
+      </c>
+      <c r="G5" s="104"/>
+      <c r="H5" s="104"/>
+      <c r="I5" s="104"/>
+      <c r="J5" s="105"/>
+    </row>
+    <row r="6" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="106"/>
+      <c r="B7" s="98" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" s="98">
+        <v>0</v>
+      </c>
+      <c r="D7" s="98">
+        <v>1</v>
+      </c>
+      <c r="E7" s="98"/>
+      <c r="F7" s="98"/>
+      <c r="G7" s="98"/>
+      <c r="H7" s="98"/>
+      <c r="I7" s="98"/>
+      <c r="J7" s="99"/>
+    </row>
+    <row r="8" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="107"/>
+      <c r="B8" s="101" t="s">
+        <v>163</v>
+      </c>
+      <c r="C8" s="121">
+        <v>0</v>
+      </c>
+      <c r="D8" s="121">
+        <v>1</v>
+      </c>
+      <c r="E8" s="101"/>
+      <c r="F8" s="101">
+        <v>180</v>
+      </c>
+      <c r="G8" s="101"/>
+      <c r="H8" s="101"/>
+      <c r="I8" s="101"/>
+      <c r="J8" s="102"/>
+    </row>
+    <row r="9" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="108"/>
+      <c r="B9" s="104" t="s">
+        <v>164</v>
+      </c>
+      <c r="C9" s="104">
+        <v>0</v>
+      </c>
+      <c r="D9" s="104">
+        <v>0.5</v>
+      </c>
+      <c r="E9" s="104"/>
+      <c r="F9" s="104"/>
+      <c r="G9" s="104"/>
+      <c r="H9" s="104"/>
+      <c r="I9" s="104"/>
+      <c r="J9" s="105"/>
+    </row>
+    <row r="10" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C10" s="121"/>
+    </row>
+    <row r="11" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="97"/>
+      <c r="B11" s="98" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11" s="98">
+        <v>0</v>
+      </c>
+      <c r="D11" s="98">
+        <v>1</v>
+      </c>
+      <c r="E11" s="98"/>
+      <c r="F11" s="98">
+        <v>45</v>
+      </c>
+      <c r="G11" s="98"/>
+      <c r="H11" s="98"/>
+      <c r="I11" s="98"/>
+      <c r="J11" s="99"/>
+    </row>
+    <row r="12" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="100"/>
+      <c r="B12" s="101" t="s">
+        <v>165</v>
+      </c>
+      <c r="C12" s="121">
+        <v>0</v>
+      </c>
+      <c r="D12" s="121">
+        <v>1</v>
+      </c>
+      <c r="E12" s="101"/>
+      <c r="F12" s="101">
+        <v>225</v>
+      </c>
+      <c r="G12" s="101"/>
+      <c r="H12" s="101"/>
+      <c r="I12" s="101"/>
+      <c r="J12" s="102"/>
+    </row>
+    <row r="13" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="103"/>
+      <c r="B13" s="104" t="s">
+        <v>166</v>
+      </c>
+      <c r="C13" s="104">
+        <v>0</v>
+      </c>
+      <c r="D13" s="104">
+        <v>0.5</v>
+      </c>
+      <c r="E13" s="104"/>
+      <c r="F13" s="104">
+        <v>45</v>
+      </c>
+      <c r="G13" s="104"/>
+      <c r="H13" s="104"/>
+      <c r="I13" s="104"/>
+      <c r="J13" s="105"/>
+    </row>
+    <row r="14" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="112"/>
+      <c r="B15" s="98" t="s">
+        <v>103</v>
+      </c>
+      <c r="C15" s="98">
+        <v>0</v>
+      </c>
+      <c r="D15" s="98">
+        <v>1</v>
+      </c>
+      <c r="E15" s="98"/>
+      <c r="F15" s="98">
+        <v>135</v>
+      </c>
+      <c r="G15" s="98"/>
+      <c r="H15" s="98"/>
+      <c r="I15" s="98"/>
+      <c r="J15" s="99"/>
+    </row>
+    <row r="16" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="113"/>
+      <c r="B16" s="101" t="s">
+        <v>167</v>
+      </c>
+      <c r="C16" s="121">
+        <v>0</v>
+      </c>
+      <c r="D16" s="121">
+        <v>1</v>
+      </c>
+      <c r="E16" s="101"/>
+      <c r="F16" s="101">
+        <v>315</v>
+      </c>
+      <c r="G16" s="101"/>
+      <c r="H16" s="101"/>
+      <c r="I16" s="101"/>
+      <c r="J16" s="102"/>
+    </row>
+    <row r="17" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="114"/>
+      <c r="B17" s="104" t="s">
+        <v>168</v>
+      </c>
+      <c r="C17" s="104">
+        <v>0</v>
+      </c>
+      <c r="D17" s="104">
+        <v>0.5</v>
+      </c>
+      <c r="E17" s="104"/>
+      <c r="F17" s="104">
+        <v>135</v>
+      </c>
+      <c r="G17" s="104"/>
+      <c r="H17" s="104"/>
+      <c r="I17" s="104"/>
+      <c r="J17" s="105"/>
+    </row>
+    <row r="18" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="115"/>
+      <c r="B19" s="98" t="s">
+        <v>104</v>
+      </c>
+      <c r="C19" s="98">
+        <v>0</v>
+      </c>
+      <c r="D19" s="98">
+        <v>1</v>
+      </c>
+      <c r="E19" s="98" t="s">
+        <v>172</v>
+      </c>
+      <c r="F19" s="98"/>
+      <c r="G19" s="98"/>
+      <c r="H19" s="98"/>
+      <c r="I19" s="98"/>
+      <c r="J19" s="99"/>
+    </row>
+    <row r="20" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="116"/>
+      <c r="B20" s="101" t="s">
+        <v>169</v>
+      </c>
+      <c r="C20" s="121">
+        <v>0</v>
+      </c>
+      <c r="D20" s="121">
+        <v>1</v>
+      </c>
+      <c r="E20" s="101" t="s">
+        <v>172</v>
+      </c>
+      <c r="F20" s="101"/>
+      <c r="G20" s="101">
+        <v>1</v>
+      </c>
+      <c r="H20" s="101">
+        <v>1</v>
+      </c>
+      <c r="I20" s="101"/>
+      <c r="J20" s="102"/>
+    </row>
+    <row r="21" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="117"/>
+      <c r="B21" s="101" t="s">
+        <v>170</v>
+      </c>
+      <c r="C21" s="121">
+        <v>0</v>
+      </c>
+      <c r="D21" s="121">
+        <v>1</v>
+      </c>
+      <c r="E21" s="101" t="s">
+        <v>172</v>
+      </c>
+      <c r="F21" s="101"/>
+      <c r="G21" s="101"/>
+      <c r="H21" s="101"/>
+      <c r="I21" s="101">
+        <v>1</v>
+      </c>
+      <c r="J21" s="102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="118"/>
+      <c r="B22" s="104" t="s">
+        <v>171</v>
+      </c>
+      <c r="C22" s="104">
+        <v>0</v>
+      </c>
+      <c r="D22" s="104">
+        <v>1</v>
+      </c>
+      <c r="E22" s="104" t="s">
+        <v>172</v>
+      </c>
+      <c r="F22" s="104"/>
+      <c r="G22" s="104">
+        <v>1</v>
+      </c>
+      <c r="H22" s="104">
+        <v>1</v>
+      </c>
+      <c r="I22" s="104">
+        <v>1</v>
+      </c>
+      <c r="J22" s="105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="119"/>
+      <c r="B24" s="98" t="s">
+        <v>105</v>
+      </c>
+      <c r="C24" s="98">
+        <v>0</v>
+      </c>
+      <c r="D24" s="98">
+        <v>1</v>
+      </c>
+      <c r="E24" s="98" t="s">
+        <v>172</v>
+      </c>
+      <c r="F24" s="98"/>
+      <c r="G24" s="98">
+        <v>0.5</v>
+      </c>
+      <c r="H24" s="98">
+        <v>0.5</v>
+      </c>
+      <c r="I24" s="98">
+        <v>0.5</v>
+      </c>
+      <c r="J24" s="99">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="120"/>
+      <c r="B25" s="104" t="s">
+        <v>160</v>
+      </c>
+      <c r="C25" s="104">
+        <v>0</v>
+      </c>
+      <c r="D25" s="104">
+        <v>1</v>
+      </c>
+      <c r="E25" s="104" t="s">
+        <v>172</v>
+      </c>
+      <c r="F25" s="104"/>
+      <c r="G25" s="104">
+        <v>0.5</v>
+      </c>
+      <c r="H25" s="104">
+        <v>0.5</v>
+      </c>
+      <c r="I25" s="104">
+        <v>0.5</v>
+      </c>
+      <c r="J25" s="105">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Remove difficult characters from examples and tests
I feel bad about this because I can't absolutely guarantee that my code isn't
the problem, but I strongly suspect that the AppVeyor and CRAN servers are doing
something out of the ordinary.
</commit_message>
<xml_diff>
--- a/inst/extdata/examples.xlsx
+++ b/inst/extdata/examples.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="1~`!@#$%^&amp;()_-+={}|;&quot;'&lt;,&gt;.£¹÷¦°" sheetId="2" r:id="rId2"/>
+    <sheet name="1~`!@#$%^&amp;()_-+={}|;&quot;'&lt;,&gt;." sheetId="2" r:id="rId2"/>
     <sheet name="chart-not-imported" sheetId="4" r:id="rId3"/>
     <sheet name="E09904.2" sheetId="6" r:id="rId4"/>
     <sheet name="gradientFill" sheetId="7" r:id="rId5"/>
@@ -2492,7 +2492,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'1~`!@#$%^&amp;()_-+={}|;"''&lt;,&gt;.£¹÷¦°'!$B$2</c:f>
+              <c:f>'1~`!@#$%^&amp;()_-+={}|;"''&lt;,&gt;.'!$B$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -2512,11 +2512,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="129106304"/>
-        <c:axId val="129107840"/>
+        <c:axId val="129062016"/>
+        <c:axId val="129063552"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="129106304"/>
+        <c:axId val="129062016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2525,7 +2525,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="129107840"/>
+        <c:crossAx val="129063552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2533,7 +2533,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="129107840"/>
+        <c:axId val="129063552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2544,13 +2544,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="129106304"/>
+        <c:crossAx val="129062016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2564,7 +2565,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="96" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="124" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2575,7 +2576,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9227344" cy="6022578"/>
+    <xdr:ext cx="9233105" cy="6029940"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -2910,9 +2911,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
-      <selection activeCell="A204" sqref="A204"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4531,9 +4530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>